<commit_message>
ntpepInfo.xlsx - small formatting changes. Appears similar to ntpepData.xlsx but missing chunks of values and yes/no values on ntpepData tab. contacts tab identical to contacts tab in ntpepData.xlsx.
</commit_message>
<xml_diff>
--- a/ntpepInfo.xlsx
+++ b/ntpepInfo.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="-160" windowWidth="24800" windowHeight="15780" activeTab="1"/>
+    <workbookView xWindow="2220" yWindow="-160" windowWidth="24800" windowHeight="15780"/>
   </bookViews>
   <sheets>
     <sheet name="ntpepInfo" sheetId="1" r:id="rId1"/>
@@ -3866,9 +3866,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:DQ55"/>
   <sheetViews>
-    <sheetView zoomScale="125" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="BG1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -14028,7 +14028,6 @@
       <c r="BU55"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <autoFilter ref="A1:DL53"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14045,7 +14044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+    <sheetView view="pageLayout" workbookViewId="0">
       <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
@@ -16630,7 +16629,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -16756,7 +16754,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -16803,7 +16800,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>